<commit_message>
AutoCommit_5 декабря 2023 г. 18:56:26_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722.xlsx
+++ b/2ИСИП-722.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1508,12 +1508,24 @@
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+      <c r="E21" s="5">
+        <v>5</v>
+      </c>
+      <c r="F21" s="5">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5">
+        <v>5</v>
+      </c>
+      <c r="H21" s="5">
+        <v>5</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5">

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 18:20:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722.xlsx
+++ b/2ИСИП-722.xlsx
@@ -545,10 +545,10 @@
   <dimension ref="A1:AN43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,9 @@
       <c r="I6" s="5">
         <v>5</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5">
+        <v>5</v>
+      </c>
       <c r="K6" s="5">
         <v>4</v>
       </c>
@@ -1312,14 +1314,30 @@
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5">
+        <v>5</v>
+      </c>
+      <c r="H14" s="5">
+        <v>5</v>
+      </c>
+      <c r="I14" s="5">
+        <v>5</v>
+      </c>
+      <c r="J14" s="5">
+        <v>10</v>
+      </c>
       <c r="K14" s="5">
         <v>4</v>
       </c>
@@ -2282,13 +2300,23 @@
       <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
+      <c r="D29" s="5">
+        <v>5</v>
+      </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="F29" s="5">
+        <v>5</v>
+      </c>
+      <c r="G29" s="5">
+        <v>5</v>
+      </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="I29" s="5">
+        <v>5</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5">
         <v>1</v>
@@ -2418,8 +2446,12 @@
       <c r="H31" s="5">
         <v>5</v>
       </c>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+      <c r="I31" s="5">
+        <v>5</v>
+      </c>
+      <c r="J31" s="5">
+        <v>5</v>
+      </c>
       <c r="K31" s="5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 18:48:52_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722.xlsx
+++ b/2ИСИП-722.xlsx
@@ -545,10 +545,10 @@
   <dimension ref="A1:AN43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -830,7 +830,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K6" s="5">
         <v>4</v>
@@ -2046,13 +2046,27 @@
       <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5">
+        <v>5</v>
+      </c>
+      <c r="E25" s="5">
+        <v>5</v>
+      </c>
+      <c r="F25" s="5">
+        <v>5</v>
+      </c>
+      <c r="G25" s="5">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>5</v>
+      </c>
+      <c r="I25" s="5">
+        <v>5</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
AutoCommit_12 декабря 2023 г. 18:50:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722.xlsx
+++ b/2ИСИП-722.xlsx
@@ -545,10 +545,10 @@
   <dimension ref="A1:AN43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1359,9 @@
       </c>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
+      <c r="R14" s="5">
+        <v>5</v>
+      </c>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>

</xml_diff>